<commit_message>
added s3 for reports
</commit_message>
<xml_diff>
--- a/src/uploads/lastLienUpload.xlsx
+++ b/src/uploads/lastLienUpload.xlsx
@@ -375,13 +375,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>block</v>
+      </c>
+      <c r="B1" t="str">
+        <v>lot</v>
+      </c>
+      <c r="C1" t="str">
+        <v>qualifier</v>
+      </c>
+      <c r="D1" t="str">
+        <v>county</v>
+      </c>
+      <c r="E1" t="str">
+        <v>address</v>
+      </c>
+      <c r="F1" t="str">
+        <v>year</v>
+      </c>
+      <c r="G1" t="str">
+        <v>llc</v>
+      </c>
+      <c r="H1" t="str">
+        <v>advertisement_number</v>
+      </c>
+      <c r="I1" t="str">
+        <v>mua_number</v>
+      </c>
+      <c r="J1" t="str">
+        <v>certificate_number</v>
+      </c>
+      <c r="K1" t="str">
+        <v>lien_type</v>
+      </c>
+      <c r="L1" t="str">
+        <v>list_item</v>
+      </c>
+      <c r="M1" t="str">
+        <v>current_owner</v>
+      </c>
+      <c r="N1" t="str">
+        <v>longitude</v>
+      </c>
+      <c r="O1" t="str">
+        <v>latitude</v>
+      </c>
+      <c r="P1" t="str">
+        <v>assessed_value</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>tax_amount</v>
+      </c>
+      <c r="R1" t="str">
+        <v>certificate_face_value</v>
+      </c>
+      <c r="S1" t="str">
+        <v>winning_bid_percentage</v>
+      </c>
+      <c r="T1" t="str">
+        <v>premium</v>
+      </c>
+      <c r="U1" t="str">
+        <v>sale_date</v>
+      </c>
+      <c r="V1" t="str">
+        <v>recording_fee</v>
+      </c>
+      <c r="W1" t="str">
+        <v>recording_date</v>
+      </c>
+      <c r="X1" t="str">
+        <v>search_fee</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2402</v>
+      </c>
+      <c r="B2" t="str">
+        <v>4.04</v>
+      </c>
+      <c r="C2" t="str">
+        <v>C0202</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="F2">
+        <v>2014</v>
+      </c>
+      <c r="G2" t="str">
+        <v>TTLBL</v>
+      </c>
+      <c r="H2">
+        <v>559</v>
+      </c>
+      <c r="I2" t="str">
+        <v>04 02402-0000-00004.04-C0202</v>
+      </c>
+      <c r="J2" t="str">
+        <v>14-00264</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Single Family Residential</v>
+      </c>
+      <c r="L2" t="str">
+        <v>C</v>
+      </c>
+      <c r="M2" t="str">
+        <v>MATTISON AVENUE PROPERTIES LLC</v>
+      </c>
+      <c r="N2">
+        <v>-74.01205</v>
+      </c>
+      <c r="O2">
+        <v>40.21634</v>
+      </c>
+      <c r="P2">
+        <v>162500</v>
+      </c>
+      <c r="Q2">
+        <v>3202.83</v>
+      </c>
+      <c r="R2">
+        <v>1105.52</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>8000</v>
+      </c>
+      <c r="U2" t="str">
+        <v>12/17/2014</v>
+      </c>
+      <c r="V2">
+        <v>30</v>
+      </c>
+      <c r="W2" t="str">
+        <v>3/9/2015</v>
+      </c>
+      <c r="X2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2402</v>
+      </c>
+      <c r="B3" t="str">
+        <v>4.05</v>
+      </c>
+      <c r="C3" t="str">
+        <v>C0301</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="F3">
+        <v>2014</v>
+      </c>
+      <c r="G3" t="str">
+        <v>TTLBL</v>
+      </c>
+      <c r="H3">
+        <v>560</v>
+      </c>
+      <c r="I3" t="str">
+        <v>04 02402-0000-00004.05-C0301</v>
+      </c>
+      <c r="J3" t="str">
+        <v>14-00265</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Single Family Residential</v>
+      </c>
+      <c r="L3" t="str">
+        <v>C</v>
+      </c>
+      <c r="M3" t="str">
+        <v>MATTISON AVENUE PROPERTIES LLC</v>
+      </c>
+      <c r="N3">
+        <v>-74.01205</v>
+      </c>
+      <c r="O3">
+        <v>40.21634</v>
+      </c>
+      <c r="P3">
+        <v>168200</v>
+      </c>
+      <c r="Q3">
+        <v>3527.88</v>
+      </c>
+      <c r="R3">
+        <v>1591.78</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>9500</v>
+      </c>
+      <c r="U3" t="str">
+        <v>12/17/2014</v>
+      </c>
+      <c r="V3">
+        <v>30</v>
+      </c>
+      <c r="W3" t="str">
+        <v>3/9/2015</v>
+      </c>
+      <c r="X3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2402</v>
+      </c>
+      <c r="B4" t="str">
+        <v>4.06</v>
+      </c>
+      <c r="C4" t="str">
+        <v>C0302</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="F4">
+        <v>2014</v>
+      </c>
+      <c r="G4" t="str">
+        <v>TTLBL</v>
+      </c>
+      <c r="H4">
+        <v>561</v>
+      </c>
+      <c r="I4" t="str">
+        <v>04 02402-0000-00004.06-C0302</v>
+      </c>
+      <c r="J4" t="str">
+        <v>14-00266</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Single Family Residential</v>
+      </c>
+      <c r="L4" t="str">
+        <v>C</v>
+      </c>
+      <c r="M4" t="str">
+        <v>MATTISON AVENUE PROPERTIES LLC</v>
+      </c>
+      <c r="N4">
+        <v>-74.01205</v>
+      </c>
+      <c r="O4">
+        <v>40.21634</v>
+      </c>
+      <c r="P4">
+        <v>169800</v>
+      </c>
+      <c r="Q4">
+        <v>3152.99</v>
+      </c>
+      <c r="R4">
+        <v>1038.23</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>8500</v>
+      </c>
+      <c r="U4" t="str">
+        <v>12/17/2014</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4" t="str">
+        <v>3/9/2015</v>
+      </c>
+      <c r="X4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2402</v>
+      </c>
+      <c r="B5" t="str">
+        <v>4.07</v>
+      </c>
+      <c r="C5" t="str">
+        <v>C0401</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="F5">
+        <v>2014</v>
+      </c>
+      <c r="G5" t="str">
+        <v>TTLBL</v>
+      </c>
+      <c r="H5">
+        <v>562</v>
+      </c>
+      <c r="I5" t="str">
+        <v>04 02402-0000-00004.07-C0401</v>
+      </c>
+      <c r="J5" t="str">
+        <v>14-00267</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Single Family Residential</v>
+      </c>
+      <c r="L5" t="str">
+        <v>C</v>
+      </c>
+      <c r="M5" t="str">
+        <v>MATTISON AVENUE PROPERTIES LLC</v>
+      </c>
+      <c r="N5">
+        <v>-74.01205</v>
+      </c>
+      <c r="O5">
+        <v>40.21634</v>
+      </c>
+      <c r="P5">
+        <v>188900</v>
+      </c>
+      <c r="Q5">
+        <v>3969.94</v>
+      </c>
+      <c r="R5">
+        <v>1909.73</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>10500</v>
+      </c>
+      <c r="U5" t="str">
+        <v>12/17/2014</v>
+      </c>
+      <c r="V5">
+        <v>30</v>
+      </c>
+      <c r="W5" t="str">
+        <v>3/9/2015</v>
+      </c>
+      <c r="X5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2402</v>
+      </c>
+      <c r="B6" t="str">
+        <v>4.08</v>
+      </c>
+      <c r="C6" t="str">
+        <v>C0402</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Asbury Park</v>
+      </c>
+      <c r="F6">
+        <v>2014</v>
+      </c>
+      <c r="G6" t="str">
+        <v>TTLBL</v>
+      </c>
+      <c r="H6">
+        <v>563</v>
+      </c>
+      <c r="I6" t="str">
+        <v>04 02402-0000-00004.08-C0402</v>
+      </c>
+      <c r="J6" t="str">
+        <v>14-00268</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Single Family Residential</v>
+      </c>
+      <c r="L6" t="str">
+        <v>C</v>
+      </c>
+      <c r="M6" t="str">
+        <v>MATTISON AVENUE PROPERTIES LLC</v>
+      </c>
+      <c r="N6">
+        <v>-74.01205</v>
+      </c>
+      <c r="O6">
+        <v>40.21634</v>
+      </c>
+      <c r="P6">
+        <v>190600</v>
+      </c>
+      <c r="Q6">
+        <v>3571.22</v>
+      </c>
+      <c r="R6">
+        <v>1334.85</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>10100</v>
+      </c>
+      <c r="U6" t="str">
+        <v>12/17/2014</v>
+      </c>
+      <c r="V6">
+        <v>30</v>
+      </c>
+      <c r="W6" t="str">
+        <v>3/9/2015</v>
+      </c>
+      <c r="X6">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>